<commit_message>
Excel files (graph 5 & 6) changed
</commit_message>
<xml_diff>
--- a/science/digital_economy_society_statistics/social_media_graph5_data.xlsx
+++ b/science/digital_economy_society_statistics/social_media_graph5_data.xlsx
@@ -44,24 +44,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>obtain</t>
-  </si>
-  <si>
-    <t>develop</t>
-  </si>
-  <si>
-    <t>recruit</t>
-  </si>
-  <si>
-    <t>exchange</t>
-  </si>
-  <si>
-    <t>involve</t>
-  </si>
-  <si>
-    <t>collaborate</t>
-  </si>
-  <si>
     <t>PC_ENT</t>
   </si>
   <si>
@@ -138,6 +120,24 @@
   </si>
   <si>
     <t>EU51</t>
+  </si>
+  <si>
+    <t>E_SM_PCUQOR</t>
+  </si>
+  <si>
+    <t>E_SM_PRCR</t>
+  </si>
+  <si>
+    <t>E_SM_PEXCHVOC</t>
+  </si>
+  <si>
+    <t>E_SM_PCUDEV</t>
+  </si>
+  <si>
+    <t>E_SM_PBPCOLL</t>
+  </si>
+  <si>
+    <t>E_SM_PADVERT</t>
   </si>
 </sst>
 </file>
@@ -467,12 +467,12 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,16 +501,16 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>2013</v>
@@ -521,16 +521,16 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2015</v>
@@ -541,16 +541,16 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>2017</v>
@@ -561,16 +561,16 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>2019</v>
@@ -581,16 +581,16 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
       </c>
       <c r="F6">
         <v>2013</v>
@@ -601,16 +601,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
       </c>
       <c r="F7">
         <v>2015</v>
@@ -621,16 +621,16 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>2017</v>
@@ -641,16 +641,16 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F9">
         <v>2019</v>
@@ -661,16 +661,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F10">
         <v>2013</v>
@@ -681,16 +681,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F11">
         <v>2015</v>
@@ -701,16 +701,16 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F12">
         <v>2017</v>
@@ -721,16 +721,16 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>2019</v>
@@ -741,16 +741,16 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F14">
         <v>2013</v>
@@ -761,16 +761,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F15">
         <v>2015</v>
@@ -781,16 +781,16 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F16">
         <v>2017</v>
@@ -801,16 +801,16 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F17">
         <v>2019</v>
@@ -821,16 +821,16 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>2013</v>
@@ -841,16 +841,16 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F19">
         <v>2015</v>
@@ -861,16 +861,16 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F20">
         <v>2017</v>
@@ -881,16 +881,16 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F21">
         <v>2019</v>
@@ -901,16 +901,16 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F22">
         <v>2013</v>
@@ -921,16 +921,16 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F23">
         <v>2015</v>
@@ -941,16 +941,16 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F24">
         <v>2017</v>
@@ -961,16 +961,16 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F25">
         <v>2019</v>

</xml_diff>